<commit_message>
Normalization finish, database completed
Database finish
</commit_message>
<xml_diff>
--- a/documents/planning/normalisation/Normalisation.xlsx
+++ b/documents/planning/normalisation/Normalisation.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="130">
   <si>
     <t>voornaam</t>
   </si>
@@ -403,12 +403,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>border_value_variable</t>
-  </si>
-  <si>
-    <t>border_value_number</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -457,9 +451,6 @@
     <t>exceedings_per_cargo_id</t>
   </si>
   <si>
-    <t>exceedings_PER_CARGO</t>
-  </si>
-  <si>
     <t>*=&gt; exceedings_per_cargo</t>
   </si>
   <si>
@@ -470,6 +461,18 @@
   </si>
   <si>
     <t>employee_stop</t>
+  </si>
+  <si>
+    <t>border_value</t>
+  </si>
+  <si>
+    <t>BORDER_PER_PRODUCT</t>
+  </si>
+  <si>
+    <t>STABILISATIONS_PER_CARGO</t>
+  </si>
+  <si>
+    <t>EXCEEDINGS_PER_CARGO</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
   <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +889,7 @@
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -905,7 +908,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -937,7 +940,7 @@
         <v>93</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -948,7 +951,7 @@
         <v>88</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H6" t="s">
         <v>98</v>
@@ -956,13 +959,13 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H7" t="s">
         <v>99</v>
@@ -973,10 +976,10 @@
         <v>102</v>
       </c>
       <c r="H8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -994,8 +997,11 @@
       <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -1011,8 +1017,14 @@
       <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>50</v>
@@ -1025,13 +1037,19 @@
       <c r="D12" t="s">
         <v>105</v>
       </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="H12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>106</v>
+      <c r="F13" t="s">
+        <v>126</v>
       </c>
       <c r="H13" t="s">
         <v>97</v>
@@ -1041,9 +1059,6 @@
       <c r="B14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D14" t="s">
-        <v>107</v>
-      </c>
       <c r="H14" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1075,24 +1090,24 @@
         <v>50</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
         <v>105</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>50</v>
@@ -1118,10 +1133,10 @@
         <v>33</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1129,16 +1144,16 @@
         <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1163,7 +1178,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1171,7 +1186,7 @@
         <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>50</v>
@@ -1199,7 +1214,7 @@
         <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1213,7 +1228,7 @@
         <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -1221,7 +1236,7 @@
         <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1231,7 +1246,7 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -1246,7 +1261,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>